<commit_message>
Version completada hasta cotizaciones con impresion, antes de guardar cambios de estatus
</commit_message>
<xml_diff>
--- a/SAGM_PROCESOS.xlsx
+++ b/SAGM_PROCESOS.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manol\Documents\PROYECTOS\SAGM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56991F7E-C125-45F1-8171-C6F7391C18E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD91B77-4C12-4975-AFB6-C854A6C5100D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="MIGRACIONES DE FRAMEWORK" sheetId="2" r:id="rId2"/>
+    <sheet name="Reports" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>LA COTIZACION TENDRA LOS SIGUIENTES ESTATUS</t>
   </si>
@@ -74,6 +75,30 @@
   </si>
   <si>
     <t>e ir a upgrade</t>
+  </si>
+  <si>
+    <t>Para trabajar con RDLC y Reportes es necesario tomar en cuenta lo siguiente</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>Hasta feb del 2024 ReportViewer no funcionaba con .NetCore por lo que fue necesario primero crear un nuevo proyecto</t>
+  </si>
+  <si>
+    <t>Que tenga un ambiente para diseñar el reporte y esto lo conseguimos con WindowsForm App (.NET Framework) con .Net Framework 4.7.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como referencia el video </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=41RcaFPphTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2) </t>
+  </si>
+  <si>
+    <t>Bajar Microsoft RDLC Report Designer si es que no lo tenemos</t>
   </si>
 </sst>
 </file>
@@ -521,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D6BC18-D9CA-4C4B-9EEB-75975C1EE3D6}">
   <dimension ref="C2:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -541,4 +566,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1509BCCB-6DB1-427E-A9D6-734794E107F1}">
+  <dimension ref="C2:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
todo listo hasta antes de Ordenes de compra
</commit_message>
<xml_diff>
--- a/SAGM_PROCESOS.xlsx
+++ b/SAGM_PROCESOS.xlsx
@@ -1,33 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manol\Documents\PROYECTOS\SAGM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD91B77-4C12-4975-AFB6-C854A6C5100D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6D6B52-7018-4B5D-94BF-9665744BCEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="MIGRACIONES DE FRAMEWORK" sheetId="2" r:id="rId2"/>
     <sheet name="Reports" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>LA COTIZACION TENDRA LOS SIGUIENTES ESTATUS</t>
   </si>
@@ -99,6 +110,18 @@
   </si>
   <si>
     <t>Bajar Microsoft RDLC Report Designer si es que no lo tenemos</t>
+  </si>
+  <si>
+    <t>3)</t>
+  </si>
+  <si>
+    <t>Para la tabla de WorkOrderDetails el registro estara completo Completed = 1 cuado</t>
+  </si>
+  <si>
+    <t>Quantity = RawMaterial = Machined = Invoiced = Shipped</t>
+  </si>
+  <si>
+    <t>El TT no intervinene porque ese es solo informativo y sirve para saber si lleva TT o no</t>
   </si>
 </sst>
 </file>
@@ -570,10 +593,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1509BCCB-6DB1-427E-A9D6-734794E107F1}">
-  <dimension ref="C2:G6"/>
+  <dimension ref="C2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -612,6 +635,24 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completo hasta formato de Cotización y se mejora el rendimiento de cotización
</commit_message>
<xml_diff>
--- a/SAGM_PROCESOS.xlsx
+++ b/SAGM_PROCESOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manol\Documents\PROYECTOS\SAGM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6D6B52-7018-4B5D-94BF-9665744BCEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E1B401-D2CB-4AB7-8A12-B7AFF9F3A325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>LA COTIZACION TENDRA LOS SIGUIENTES ESTATUS</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>El TT no intervinene porque ese es solo informativo y sirve para saber si lleva TT o no</t>
+  </si>
+  <si>
+    <t>INSTALACION Chart.js</t>
+  </si>
+  <si>
+    <t>se instala desde consola de NPM y despues vas a "C:\Users\manol\.nuget\packages\chart.js\3.7.1\content\Scripts"</t>
+  </si>
+  <si>
+    <t>y copiamos la librería</t>
   </si>
 </sst>
 </file>
@@ -488,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:D10"/>
+  <dimension ref="C3:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,6 +569,19 @@
         <v>13</v>
       </c>
     </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -569,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D6BC18-D9CA-4C4B-9EEB-75975C1EE3D6}">
   <dimension ref="C2:C3"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -595,7 +617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1509BCCB-6DB1-427E-A9D6-734794E107F1}">
   <dimension ref="C2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>